<commit_message>
create : test object , completed course crud update : idNameMap to idUserMap
</commit_message>
<xml_diff>
--- a/TrainingModuleExcelSearch/Training Plan/Rakesh Kumar/Unreal.xlsx
+++ b/TrainingModuleExcelSearch/Training Plan/Rakesh Kumar/Unreal.xlsx
@@ -9,17 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="AqI8TiX9MhPrOuxy3kvumWf2uofW+EZ0AKZXNsxD2EM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="ZBN/I3t33g8+M3mOk1c+zrgpwqT72Vs2DuxJcMGU/Vw="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
-  <si>
-    <t>Unreal Training Plan</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Phase</t>
   </si>
@@ -379,7 +376,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
@@ -388,21 +385,14 @@
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <sz val="12.0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font/>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -416,12 +406,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
+    <font/>
     <font>
       <u/>
       <sz val="10.0"/>
@@ -432,12 +417,6 @@
       <u/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -461,42 +440,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -541,69 +490,42 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -821,348 +743,339 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="12.56"/>
+    <col customWidth="1" min="1" max="1" width="12.56"/>
+    <col customWidth="1" min="2" max="2" width="19.0"/>
     <col customWidth="1" min="3" max="3" width="36.78"/>
     <col customWidth="1" min="4" max="4" width="10.89"/>
     <col customWidth="1" min="5" max="5" width="31.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="9">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5">
         <v>8.0</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>9</v>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="13">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5">
         <v>8.0</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>11</v>
+      <c r="E4" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="13">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5">
         <v>8.0</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="13">
+      <c r="E6" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5">
         <v>24.0</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="11"/>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="E7" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="5">
         <v>8.0</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="13">
+      <c r="E9" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7"/>
+      <c r="B10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8"/>
+      <c r="B11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5">
+        <v>12.0</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5">
+        <v>16.0</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8"/>
+      <c r="B13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8"/>
+      <c r="B15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="5">
+        <v>32.0</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5">
         <v>24.0</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="13">
-        <v>24.0</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="11"/>
-      <c r="B10" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="13">
-        <v>8.0</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="11"/>
-      <c r="B11" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="13">
-        <v>20.0</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="15"/>
-      <c r="B12" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="13">
-        <v>12.0</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="13">
+      <c r="E16" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8"/>
+      <c r="B17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="5">
         <v>16.0</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="15"/>
-      <c r="B14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="13">
-        <v>8.0</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="13">
-        <v>20.0</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="15"/>
-      <c r="B16" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="13">
+      <c r="E17" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="5">
         <v>32.0</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="9">
-        <v>24.0</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="15"/>
-      <c r="B18" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="9">
+      <c r="E18" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8"/>
+      <c r="B19" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="5">
         <v>16.0</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="13">
-        <v>32.0</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="15"/>
-      <c r="B20" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="E19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="9">
-        <v>16.0</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>62</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B7:B8"/>
+  <mergeCells count="9">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E3"/>
-    <hyperlink r:id="rId2" ref="E4"/>
-    <hyperlink r:id="rId3" ref="E5"/>
-    <hyperlink r:id="rId4" ref="E6"/>
-    <hyperlink r:id="rId5" ref="E7"/>
-    <hyperlink r:id="rId6" ref="E8"/>
-    <hyperlink r:id="rId7" ref="E9"/>
-    <hyperlink r:id="rId8" ref="E10"/>
-    <hyperlink r:id="rId9" ref="E11"/>
-    <hyperlink r:id="rId10" ref="E12"/>
-    <hyperlink r:id="rId11" ref="E13"/>
-    <hyperlink r:id="rId12" ref="E14"/>
-    <hyperlink r:id="rId13" ref="E15"/>
-    <hyperlink r:id="rId14" ref="E16"/>
-    <hyperlink r:id="rId15" ref="E17"/>
-    <hyperlink r:id="rId16" ref="E18"/>
-    <hyperlink r:id="rId17" ref="E19"/>
-    <hyperlink r:id="rId18" ref="E20"/>
+    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink r:id="rId2" ref="E3"/>
+    <hyperlink r:id="rId3" ref="E4"/>
+    <hyperlink r:id="rId4" ref="E5"/>
+    <hyperlink r:id="rId5" ref="E6"/>
+    <hyperlink r:id="rId6" ref="E7"/>
+    <hyperlink r:id="rId7" ref="E8"/>
+    <hyperlink r:id="rId8" ref="E9"/>
+    <hyperlink r:id="rId9" ref="E10"/>
+    <hyperlink r:id="rId10" ref="E11"/>
+    <hyperlink r:id="rId11" ref="E12"/>
+    <hyperlink r:id="rId12" ref="E13"/>
+    <hyperlink r:id="rId13" ref="E14"/>
+    <hyperlink r:id="rId14" ref="E15"/>
+    <hyperlink r:id="rId15" ref="E16"/>
+    <hyperlink r:id="rId16" ref="E17"/>
+    <hyperlink r:id="rId17" ref="E18"/>
+    <hyperlink r:id="rId18" ref="E19"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>

</xml_diff>